<commit_message>
Almost finished testbed CAD, doing alternate
More or less done with the actuator assemblies, and made an assembly
with the sliding masses, with the z-axis smack-dab in the middle. I want
to make an alternate one where the z-axis is on the side. Committing now
because saving a bunch of copies might mess up my SW references.
</commit_message>
<xml_diff>
--- a/hardware/Orders/PR_McMaster.xlsx
+++ b/hardware/Orders/PR_McMaster.xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">PR!$A$1:$L$62</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">PR!$A$1:$L$62</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">PR!$A$1:$L$62</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">PR!$A$1:$L$62</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -1889,7 +1890,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2005,7 +2006,7 @@
   <dimension ref="A1:AF139"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="A43:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3724,7 +3725,7 @@
   <dimension ref="A2:B39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+      <selection pane="topLeft" activeCell="A39" activeCellId="1" sqref="A43:B43 A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>